<commit_message>
Updated few descriptions and default model. Slight changes to json
</commit_message>
<xml_diff>
--- a/URLS.xlsx
+++ b/URLS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://armeta-my.sharepoint.com/personal/jonathan_white_armeta_com/Documents/Documents/Internal/AI_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonathanWhite\source\repos\SkillsDev2\Skills Development Project - Phase II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="558" documentId="8_{061D8BA6-4A7F-4BE0-AC67-2FC4DD546879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8FCCECA-5AB1-4256-A425-26FE60625B87}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CE0B4B-8418-40E7-AD0A-0A57EC4BC627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{B46CBADC-52FD-4FC8-8DE4-4CF8F89977F2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{B46CBADC-52FD-4FC8-8DE4-4CF8F89977F2}"/>
   </bookViews>
   <sheets>
     <sheet name="URLs" sheetId="1" r:id="rId1"/>
@@ -563,10 +563,10 @@
     <t>Insights about user interaction across channels</t>
   </si>
   <si>
-    <t>displaying the types and times of engagements</t>
-  </si>
-  <si>
-    <t>relating the conversion rate of users to actions and times in order to maximize revenue</t>
+    <t>displaying the types and times of user engagements including registrations, offer view, and redemptions</t>
+  </si>
+  <si>
+    <t>relating the conversion rate of users through mobile event steps to specific offers and times in order to maximize revenue and the conversion rate</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2159,7 @@
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>'Filled In'!A43</f>
-        <v>Insights about user interaction across channels relating the conversion rate of users to actions and times in order to maximize revenue</v>
+        <v>Insights about user interaction across channels relating the conversion rate of users through mobile event steps to specific offers and times in order to maximize revenue and the conversion rate</v>
       </c>
       <c r="B43" t="s">
         <v>166</v>
@@ -2174,7 +2174,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>'Filled In'!A44</f>
-        <v>Insights about user interaction across channels displaying the types and times of engagements</v>
+        <v>Insights about user interaction across channels displaying the types and times of user engagements including registrations, offer view, and redemptions</v>
       </c>
       <c r="B44" t="s">
         <v>167</v>
@@ -2198,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38015EBD-3507-4B60-BF02-A944042A0F68}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6386,10 +6386,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f>_xlfn.CONCAT(C43, " ",D43)</f>
-        <v>Insights about user interaction across channels relating the conversion rate of users to actions and times in order to maximize revenue</v>
+        <v>Insights about user interaction across channels relating the conversion rate of users through mobile event steps to specific offers and times in order to maximize revenue and the conversion rate</v>
       </c>
       <c r="B43" t="str">
         <f>URLs!B43</f>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="D43" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(D$1,"_",URLs!D43),Descs!$A$2:$A$60, Descs!$D$2:$D$60)</f>
-        <v>relating the conversion rate of users to actions and times in order to maximize revenue</v>
+        <v>relating the conversion rate of users through mobile event steps to specific offers and times in order to maximize revenue and the conversion rate</v>
       </c>
       <c r="E43" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(E$1,"_",URLs!E43),Descs!$A$2:$A$60, Descs!$D$2:$D$60)</f>
@@ -6467,7 +6467,7 @@
     <row r="44" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f>_xlfn.CONCAT(C44, " ",D44)</f>
-        <v>Insights about user interaction across channels displaying the types and times of engagements</v>
+        <v>Insights about user interaction across channels displaying the types and times of user engagements including registrations, offer view, and redemptions</v>
       </c>
       <c r="B44" t="str">
         <f>URLs!B44</f>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="D44" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(D$1,"_",URLs!D44),Descs!$A$2:$A$60, Descs!$D$2:$D$60)</f>
-        <v>displaying the types and times of engagements</v>
+        <v>displaying the types and times of user engagements including registrations, offer view, and redemptions</v>
       </c>
       <c r="E44" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(E$1,"_",URLs!E44),Descs!$A$2:$A$60, Descs!$D$2:$D$60)</f>
@@ -6551,14 +6551,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0AE4062-F6EB-4483-B178-974DF29C2A75}">
   <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT("{""options"": [", _xlfn.TEXTJOIN(", ",TRUE, A2:A44), "]}")</f>
-        <v>{"options": [{"url": "https://ip.armeta.com/demo/analytics/sales-opportunity", "desc": "Insights about sales data that compares sale opportunity of unsold all product types across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjB9", "desc": "Insights about sales data that compares sale opportunity of unsold other product types across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjF9", "desc": "Insights about sales data that compares sale opportunity of unsold mens products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjN9", "desc": "Insights about sales data that compares sale opportunity of unsold womens products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjR9", "desc": "Insights about sales data that compares sale opportunity of unsold juniors products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjV9", "desc": "Insights about sales data that compares sale opportunity of unsold childrens products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjZ9", "desc": "Insights about sales data that compares sale opportunity of unsold cosmetic products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjd9", "desc": "Insights about sales data that compares sale opportunity of unsold accessory products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjh9", "desc": "Insights about sales data that compares sale opportunity of unsold mens and womens shoes across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjl9", "desc": "Insights about sales data that compares sale opportunity of unsold hard and soft home products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: year to date, from the start of the current year to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: year to date, from the start of the current year to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJkb2xsYXJzIiwidGltZWZyYW1lIjoiTVREIn0%3D", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: month to date, from the start of the month to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyIsInRpbWVmcmFtZSI6Ik1URCJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: month to date, from the start of the month to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJkb2xsYXJzIiwidGltZWZyYW1lIjoiV1REIn0%3D", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: week to date, from the start of the week to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyIsInRpbWVmcmFtZSI6IldURCJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: week to date, from the start of the week to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJkb2xsYXJzIiwidGltZWZyYW1lIjoiREFZIn0%3D", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: from yesterday within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyIsInRpbWVmcmFtZSI6IkRBWSJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: from yesterday within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of year to date, from the start of the current year to today and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product?query=eyJ0aW1lZnJhbWUiOiJNVEQifQ%3D%3D", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of month to date, from the start of the month to today and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product?query=eyJ0aW1lZnJhbWUiOiJXVEQifQ%3D%3D", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of week to date, from the start of the week to today and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product?query=eyJ0aW1lZnJhbWUiOiJEQVkifQ%3D%3D", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of from yesterday and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within all industries. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkNvbnN1bWVyIFByb2R1Y3RzIn0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the consumer products industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkZpbmFuY2lhbCBTZXJ2aWNlcyJ9", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the financial services industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkdvdmVybm1lbnQifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the government industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkhlYWx0aGNhcmUifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the healthcare industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6Ikluc3VyYW5jZSJ9", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the insurance industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6Ik1hbnVmYWN0dXJpbmcifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the manufacturing industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlBoYXJtYWNldXRpY2FsIn0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the pharmaceutical industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlJldGFpbCAmIGVDb21tZXJjZSJ9", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the retail &amp; ecommerce industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlNlcnZpY2VzIn0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the services industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlRlY2hub2xvZ3kifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the technology industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlRlbGVjb20ifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the telecom industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlRyYXZlbCAmIEhvc3BpdGFsaXR5In0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the travel &amp; hostpitality industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlV0aWxpdHkifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the utility industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/location-review", "desc": "Insights about sales data, specifically sales and inventory for specific locations and stores in eastern states, new england, east coast, atlantic. Data aggregated at the timescale of month to date, from the start of the month to this current week from all groups and all families", "encoding": null, "category": "Sales Accelerator", "page": "Location Review"}, {"url": "https://ip.armeta.com/demo/analytics/location-review?query=eyJ3ZWVrIjoiTFcifQ%3D%3D", "desc": "Insights about sales data, specifically sales and inventory for specific locations and stores in eastern states, new england, east coast, atlantic. Data aggregated at the timescale of month to date, from the start of the month to the past week, the last week from all groups and all families", "encoding": null, "category": "Sales Accelerator", "page": "Location Review"}, {"url": "https://ip.armeta.com/demo/analytics/top-styles", "desc": "Insights about sales data highlighting the top products at middletown, west virginia during the timeframe of month to date, from the start of the month to this current week from all families", "encoding": null, "category": "Sales Accelerator", "page": "Top Styles"}, {"url": "https://ip.armeta.com/demo/analytics/optical-analysis-sales", "desc": "Insights about optical sales, such as frames and lenses, aggregated by eye care metrics over the timespan of year to date, from the start of the current year to today across all locations and all positions", "encoding": null, "category": "Optical Demo", "page": "Optical Demo Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/optical-analysis-product", "desc": "Insights about optical sales, such as frames and lenses, analyizing product makeup of orders over the timespan of year to date, from the start of the current year to today across all locations and all positions", "encoding": null, "category": "Optical Demo", "page": "Lens Producr Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/conversion-maximizer", "desc": "Insights about user interaction across channels relating the conversion rate of users to actions and times in order to maximize revenue", "encoding": null, "category": "Omnichannel Drivers", "page": "Conversion Maximizer"}, {"url": "https://ip.armeta.com/demo/analytics/mobile-engagement", "desc": "Insights about user interaction across channels displaying the types and times of engagements", "encoding": null, "category": "Omnichannel Drivers", "page": "Mobile Engagement"}]}</v>
+        <v>{"options": [{"url": "https://ip.armeta.com/demo/analytics/sales-opportunity", "desc": "Insights about sales data that compares sale opportunity of unsold all product types across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjB9", "desc": "Insights about sales data that compares sale opportunity of unsold other product types across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjF9", "desc": "Insights about sales data that compares sale opportunity of unsold mens products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjN9", "desc": "Insights about sales data that compares sale opportunity of unsold womens products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjR9", "desc": "Insights about sales data that compares sale opportunity of unsold juniors products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjV9", "desc": "Insights about sales data that compares sale opportunity of unsold childrens products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjZ9", "desc": "Insights about sales data that compares sale opportunity of unsold cosmetic products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjd9", "desc": "Insights about sales data that compares sale opportunity of unsold accessory products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjh9", "desc": "Insights about sales data that compares sale opportunity of unsold mens and womens shoes across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-opportunity?query=eyJmYW1pbHkiOjl9", "desc": "Insights about sales data that compares sale opportunity of unsold hard and soft home products across all groups within all states, america, national, nationwide", "encoding": null, "category": "Sales Accelerator", "page": "Sales Opportunity"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: year to date, from the start of the current year to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: year to date, from the start of the current year to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJkb2xsYXJzIiwidGltZWZyYW1lIjoiTVREIn0%3D", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: month to date, from the start of the month to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyIsInRpbWVmcmFtZSI6Ik1URCJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: month to date, from the start of the month to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJkb2xsYXJzIiwidGltZWZyYW1lIjoiV1REIn0%3D", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: week to date, from the start of the week to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyIsInRpbWVmcmFtZSI6IldURCJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: week to date, from the start of the week to today within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJkb2xsYXJzIiwidGltZWZyYW1lIjoiREFZIn0%3D", "desc": "Insights about sales data, the revenue in dollars aggreagted by category for a specified timeframe: from yesterday within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-retail?query=eyJtZXRyaWMiOiJ1bml0cyIsInRpbWVmcmFtZSI6IkRBWSJ9", "desc": "Insights about sales data, the number of units sold aggreagted by category for a specified timeframe: from yesterday within all locations", "encoding": null, "category": "Sales Accelerator", "page": "Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of year to date, from the start of the current year to today and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product?query=eyJ0aW1lZnJhbWUiOiJNVEQifQ%3D%3D", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of month to date, from the start of the month to today and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product?query=eyJ0aW1lZnJhbWUiOiJXVEQifQ%3D%3D", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of week to date, from the start of the week to today and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/analysis-product?query=eyJ0aW1lZnJhbWUiOiJEQVkifQ%3D%3D", "desc": "Insights about sales data to gain insight on how certain products are selling. Who and how products are sold within the timeframe of from yesterday and located in all locations and in all positions", "encoding": null, "category": "Sales Accelerator", "page": "Product Insight"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within all industries. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkNvbnN1bWVyIFByb2R1Y3RzIn0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the consumer products industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkZpbmFuY2lhbCBTZXJ2aWNlcyJ9", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the financial services industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkdvdmVybm1lbnQifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the government industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IkhlYWx0aGNhcmUifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the healthcare industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6Ikluc3VyYW5jZSJ9", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the insurance industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6Ik1hbnVmYWN0dXJpbmcifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the manufacturing industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlBoYXJtYWNldXRpY2FsIn0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the pharmaceutical industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlJldGFpbCAmIGVDb21tZXJjZSJ9", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the retail &amp; ecommerce industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlNlcnZpY2VzIn0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the services industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlRlY2hub2xvZ3kifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the technology industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlRlbGVjb20ifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the telecom industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlRyYXZlbCAmIEhvc3BpdGFsaXR5In0%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the travel &amp; hostpitality industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/sales-digital?query=eyJpbmR1c3RyeSI6IlV0aWxpdHkifQ%3D%3D", "desc": "Insights about sales data from digital website metrics, such as conversion rate and average order value by site, within the utility industry. Data compared against the market across all volumes and all types and all clients as US dollars", "encoding": null, "category": "Sales Accelerator", "page": "Digital Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/location-review", "desc": "Insights about sales data, specifically sales and inventory for specific locations and stores in eastern states, new england, east coast, atlantic. Data aggregated at the timescale of month to date, from the start of the month to this current week from all groups and all families", "encoding": null, "category": "Sales Accelerator", "page": "Location Review"}, {"url": "https://ip.armeta.com/demo/analytics/location-review?query=eyJ3ZWVrIjoiTFcifQ%3D%3D", "desc": "Insights about sales data, specifically sales and inventory for specific locations and stores in eastern states, new england, east coast, atlantic. Data aggregated at the timescale of month to date, from the start of the month to the past week, the last week from all groups and all families", "encoding": null, "category": "Sales Accelerator", "page": "Location Review"}, {"url": "https://ip.armeta.com/demo/analytics/top-styles", "desc": "Insights about sales data highlighting the top products at middletown, west virginia during the timeframe of month to date, from the start of the month to this current week from all families", "encoding": null, "category": "Sales Accelerator", "page": "Top Styles"}, {"url": "https://ip.armeta.com/demo/analytics/optical-analysis-sales", "desc": "Insights about optical sales, such as frames and lenses, aggregated by eye care metrics over the timespan of year to date, from the start of the current year to today across all locations and all positions", "encoding": null, "category": "Optical Demo", "page": "Optical Demo Sales Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/optical-analysis-product", "desc": "Insights about optical sales, such as frames and lenses, analyizing product makeup of orders over the timespan of year to date, from the start of the current year to today across all locations and all positions", "encoding": null, "category": "Optical Demo", "page": "Lens Producr Analysis"}, {"url": "https://ip.armeta.com/demo/analytics/conversion-maximizer", "desc": "Insights about user interaction across channels relating the conversion rate of users through mobile event steps to specific offers and times in order to maximize revenue and the conversion rate", "encoding": null, "category": "Omnichannel Drivers", "page": "Conversion Maximizer"}, {"url": "https://ip.armeta.com/demo/analytics/mobile-engagement", "desc": "Insights about user interaction across channels displaying the types and times of user engagements including registrations, offer view, and redemptions", "encoding": null, "category": "Omnichannel Drivers", "page": "Mobile Engagement"}]}</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -6810,13 +6810,13 @@
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>_xlfn.CONCAT("{""url"": """, URLs!B43, """, ""desc"": """, URLs!A43, """, ""encoding"": null, ""category"": """, URLs!C43, """, ""page"": """, URLs!D43, """}")</f>
-        <v>{"url": "https://ip.armeta.com/demo/analytics/conversion-maximizer", "desc": "Insights about user interaction across channels relating the conversion rate of users to actions and times in order to maximize revenue", "encoding": null, "category": "Omnichannel Drivers", "page": "Conversion Maximizer"}</v>
+        <v>{"url": "https://ip.armeta.com/demo/analytics/conversion-maximizer", "desc": "Insights about user interaction across channels relating the conversion rate of users through mobile event steps to specific offers and times in order to maximize revenue and the conversion rate", "encoding": null, "category": "Omnichannel Drivers", "page": "Conversion Maximizer"}</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>_xlfn.CONCAT("{""url"": """, URLs!B44, """, ""desc"": """, URLs!A44, """, ""encoding"": null, ""category"": """, URLs!C44, """, ""page"": """, URLs!D44, """}")</f>
-        <v>{"url": "https://ip.armeta.com/demo/analytics/mobile-engagement", "desc": "Insights about user interaction across channels displaying the types and times of engagements", "encoding": null, "category": "Omnichannel Drivers", "page": "Mobile Engagement"}</v>
+        <v>{"url": "https://ip.armeta.com/demo/analytics/mobile-engagement", "desc": "Insights about user interaction across channels displaying the types and times of user engagements including registrations, offer view, and redemptions", "encoding": null, "category": "Omnichannel Drivers", "page": "Mobile Engagement"}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>